<commit_message>
[アセットマネジメント] [add field] scinario_03
</commit_message>
<xml_diff>
--- a/app/seeds/asset.xlsx
+++ b/app/seeds/asset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>名前</t>
   </si>
@@ -254,6 +254,17 @@
   </si>
   <si>
     <t>test_101.zip</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>asset_info</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アセット情報</t>
+    <rPh sb="4" eb="6">
+      <t>ジョウホウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -341,8 +352,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -378,7 +395,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="29">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -390,6 +407,9 @@
     <cellStyle name="ハイパーリンク" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -402,6 +422,9 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="28" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -735,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E17" sqref="E17:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -887,82 +910,107 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="6" t="s">
+    <row r="16" spans="1:6">
+      <c r="A16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="2">
+    <row r="17" spans="1:6">
+      <c r="A17" s="2">
         <v>10001001</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B17" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="C16" s="7">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="2">
-        <v>10001002</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="C17" s="7">
         <v>1</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2">
+        <v>10001002</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
+      <c r="E18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5">
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5">
-      <c r="E22" s="8" t="s">
+    <row r="22" spans="1:6">
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="E23" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="E23" s="9" t="s">
+    <row r="24" spans="1:6">
+      <c r="E24" s="9" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[アセットマネジメント] [edit field] scinario_04
</commit_message>
<xml_diff>
--- a/app/seeds/asset.xlsx
+++ b/app/seeds/asset.xlsx
@@ -761,7 +761,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:E18"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -888,7 +888,9 @@
       <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
       <c r="E11" s="7" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
[アセットマネジメント] [delete field] scinario_05
</commit_message>
<xml_diff>
--- a/app/seeds/asset.xlsx
+++ b/app/seeds/asset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>名前</t>
   </si>
@@ -254,17 +254,6 @@
   </si>
   <si>
     <t>test_101.zip</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>asset_info</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>アセット情報</t>
-    <rPh sb="4" eb="6">
-      <t>ジョウホウ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -758,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E15" sqref="E15:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -888,9 +877,7 @@
       <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="6">
-        <v>1</v>
-      </c>
+      <c r="D11" s="6"/>
       <c r="E11" s="7" t="s">
         <v>27</v>
       </c>
@@ -912,107 +899,82 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="2"/>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>15</v>
+      <c r="A15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="6" t="s">
-        <v>21</v>
+      <c r="A16" s="2">
+        <v>10001001</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>39</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="2">
-        <v>10001001</v>
+        <v>10001002</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C17" s="7">
         <v>1</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="2">
-        <v>10001002</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="7">
-        <v>1</v>
-      </c>
-      <c r="D18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
         <v>38</v>
       </c>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5">
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:5">
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:5">
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:6">
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="E23" s="8" t="s">
+    <row r="22" spans="1:5">
+      <c r="E22" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
-      <c r="E24" s="9" t="s">
+    <row r="23" spans="1:5">
+      <c r="E23" s="9" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[アセットマネジメント] [add data] scinario_06
</commit_message>
<xml_diff>
--- a/app/seeds/asset.xlsx
+++ b/app/seeds/asset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>名前</t>
   </si>
@@ -254,6 +254,14 @@
   </si>
   <si>
     <t>test_101.zip</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メニューアセット2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>test_102.zip</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -341,8 +349,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -384,7 +398,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="35">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -399,6 +413,9 @@
     <cellStyle name="ハイパーリンク" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -414,6 +431,9 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="34" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -750,7 +770,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:E17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -954,12 +974,24 @@
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" t="s">
+      <c r="A18" s="2">
+        <v>10001003</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5">
       <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5">

</xml_diff>

<commit_message>
[アセットマネジメント] [edit data] scinario_07
</commit_message>
<xml_diff>
--- a/app/seeds/asset.xlsx
+++ b/app/seeds/asset.xlsx
@@ -770,7 +770,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -981,7 +981,7 @@
         <v>41</v>
       </c>
       <c r="C18" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
[アセットマネジメント] [delete data] scinario_08
</commit_message>
<xml_diff>
--- a/app/seeds/asset.xlsx
+++ b/app/seeds/asset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>名前</t>
   </si>
@@ -254,14 +254,6 @@
   </si>
   <si>
     <t>test_101.zip</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>メニューアセット2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>test_102.zip</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -767,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -974,39 +966,24 @@
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="2">
-        <v>10001003</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="7">
-        <v>2</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>42</v>
+      <c r="A18" t="s">
+        <v>38</v>
       </c>
       <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>38</v>
-      </c>
       <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5">
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="E21" s="8"/>
+      <c r="E21" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="E22" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="E23" s="9" t="s">
+      <c r="E22" s="9" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>